<commit_message>
Added links to homeworks on Facebook & GitHub
</commit_message>
<xml_diff>
--- a/storage/costs/Koszty.xlsx
+++ b/storage/costs/Koszty.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karolina/IdeaProjects/azure-architecture-homeworks/storage/costs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE0A789-086B-B540-8D12-084DDA3482EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD06587D-E6D4-5A42-BC53-BE2D38D4999A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="36880" windowHeight="20620" activeTab="2" xr2:uid="{E8F46193-524B-C040-894E-EE829788C2D1}"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{E8F46193-524B-C040-894E-EE829788C2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="DETAILS" sheetId="5" r:id="rId1"/>
     <sheet name="DETAILS_OLD" sheetId="2" r:id="rId2"/>
     <sheet name="SUMMARY" sheetId="4" r:id="rId3"/>
-    <sheet name="RA-GRS" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="RA-GRS" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="98">
   <si>
     <t>Utworzenie backupu</t>
   </si>
@@ -952,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09DED91-B716-A847-992F-C4E4880362FA}">
   <dimension ref="A2:J106"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,11 +1054,11 @@
         <v>0</v>
       </c>
       <c r="G9" s="29">
-        <f>F9*C9</f>
+        <f t="shared" ref="G9:G14" si="0">F9*C9</f>
         <v>0</v>
       </c>
       <c r="H9" s="14">
-        <f>B9*C9</f>
+        <f t="shared" ref="H9:H14" si="1">B9*C9</f>
         <v>365</v>
       </c>
       <c r="I9" s="17"/>
@@ -1076,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="14">
-        <f t="shared" ref="E10:E14" si="0">D10*B10</f>
+        <f t="shared" ref="E10:E14" si="2">D10*B10</f>
         <v>365</v>
       </c>
       <c r="F10" s="29">
@@ -1084,11 +1085,11 @@
         <v>1</v>
       </c>
       <c r="G10" s="29">
-        <f>F10*C10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H10" s="14">
-        <f>B10*C10</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="I10" s="17"/>
@@ -1107,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>365</v>
       </c>
       <c r="F11" s="29">
@@ -1115,11 +1116,11 @@
         <v>2</v>
       </c>
       <c r="G11" s="29">
-        <f>F11*C11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11" s="14">
-        <f>B11*C11</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="I11" s="17"/>
@@ -1138,18 +1139,18 @@
         <v>1</v>
       </c>
       <c r="E12" s="14">
+        <f t="shared" si="2"/>
+        <v>366</v>
+      </c>
+      <c r="F12" s="29">
+        <v>2</v>
+      </c>
+      <c r="G12" s="29">
         <f t="shared" si="0"/>
-        <v>366</v>
-      </c>
-      <c r="F12" s="29">
-        <v>2</v>
-      </c>
-      <c r="G12" s="29">
-        <f>F12*C12</f>
         <v>2</v>
       </c>
       <c r="H12" s="14">
-        <f>B12*C12</f>
+        <f t="shared" si="1"/>
         <v>366</v>
       </c>
       <c r="I12" s="17"/>
@@ -1168,18 +1169,18 @@
         <v>1</v>
       </c>
       <c r="E13" s="14">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="F13" s="29">
+        <v>2</v>
+      </c>
+      <c r="G13" s="29">
         <f t="shared" si="0"/>
-        <v>365</v>
-      </c>
-      <c r="F13" s="29">
-        <v>2</v>
-      </c>
-      <c r="G13" s="29">
-        <f>F13*C13</f>
         <v>2</v>
       </c>
       <c r="H13" s="14">
-        <f>B13*C13</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="I13" s="17"/>
@@ -1198,18 +1199,18 @@
         <v>1</v>
       </c>
       <c r="E14" s="14">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="F14" s="29">
+        <v>2</v>
+      </c>
+      <c r="G14" s="29">
         <f t="shared" si="0"/>
-        <v>365</v>
-      </c>
-      <c r="F14" s="29">
-        <v>2</v>
-      </c>
-      <c r="G14" s="29">
-        <f>F14*C14</f>
         <v>2</v>
       </c>
       <c r="H14" s="14">
-        <f>B14*C14</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="I14" s="17"/>
@@ -1314,14 +1315,14 @@
         <v>0.01</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" ref="D22:D23" si="1">C22*1000*12/365</f>
+        <f t="shared" ref="D22:D23" si="3">C22*1000*12/365</f>
         <v>0.32876712328767121</v>
       </c>
       <c r="E22" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F22" s="20">
-        <f t="shared" ref="F22:F23" si="2">E22*1000*12/365</f>
+        <f t="shared" ref="F22:F23" si="4">E22*1000*12/365</f>
         <v>0.82191780821917804</v>
       </c>
     </row>
@@ -1334,14 +1335,14 @@
         <v>2.3E-3</v>
       </c>
       <c r="D23" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.5616438356164384E-2</v>
       </c>
       <c r="E23" s="20">
         <v>4.3E-3</v>
       </c>
       <c r="F23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.14136986301369861</v>
       </c>
     </row>
@@ -1435,7 +1436,7 @@
         <v>7.5616438356164384E-2</v>
       </c>
       <c r="F29" s="15">
-        <f>E29*(((C29+D29)*B29)/2)</f>
+        <f>(((E29*C29+E29*D29))*B29)/2</f>
         <v>5050.8</v>
       </c>
       <c r="G29" s="29">
@@ -1446,7 +1447,7 @@
         <v>55.2</v>
       </c>
       <c r="I29" s="11">
-        <f t="shared" ref="I29:I34" si="3">F29-H29</f>
+        <f t="shared" ref="I29:I34" si="5">F29-H29</f>
         <v>4995.6000000000004</v>
       </c>
     </row>
@@ -1462,26 +1463,26 @@
         <v>366</v>
       </c>
       <c r="D30" s="14">
-        <f t="shared" ref="D30:D34" si="4">B30+C30-1</f>
+        <f t="shared" ref="D30:D34" si="6">B30+C30-1</f>
         <v>730</v>
       </c>
       <c r="E30" s="22">
-        <f t="shared" ref="E30:E34" si="5">$D$23</f>
+        <f t="shared" ref="E30:E34" si="7">$D$23</f>
         <v>7.5616438356164384E-2</v>
       </c>
       <c r="F30" s="15">
-        <f t="shared" ref="F30:F34" si="6">E30*(((C30+D30)*B30)/2)</f>
+        <f>(((E30*C30+E30*D30))*B30)/2</f>
         <v>15124.8</v>
       </c>
       <c r="G30" s="29">
         <v>2</v>
       </c>
       <c r="H30" s="25">
-        <f t="shared" ref="H30:H34" si="7">G30*E30*B30</f>
+        <f>G30*E30*B30</f>
         <v>55.2</v>
       </c>
       <c r="I30" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15069.599999999999</v>
       </c>
     </row>
@@ -1497,27 +1498,27 @@
         <v>731</v>
       </c>
       <c r="D31" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1095</v>
       </c>
       <c r="E31" s="22">
+        <f t="shared" si="7"/>
+        <v>7.5616438356164384E-2</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" ref="F31:F34" si="8">(((E31*C31+E31*D31))*B31)/2</f>
+        <v>25198.800000000003</v>
+      </c>
+      <c r="G31" s="29">
+        <v>2</v>
+      </c>
+      <c r="H31" s="25">
+        <f>G31*E31*B31</f>
+        <v>55.2</v>
+      </c>
+      <c r="I31" s="11">
         <f t="shared" si="5"/>
-        <v>7.5616438356164384E-2</v>
-      </c>
-      <c r="F31" s="15">
-        <f t="shared" si="6"/>
-        <v>25198.799999999999</v>
-      </c>
-      <c r="G31" s="29">
-        <v>2</v>
-      </c>
-      <c r="H31" s="25">
-        <f t="shared" si="7"/>
-        <v>55.2</v>
-      </c>
-      <c r="I31" s="11">
-        <f t="shared" si="3"/>
-        <v>25143.599999999999</v>
+        <v>25143.600000000002</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1532,26 +1533,26 @@
         <v>731</v>
       </c>
       <c r="D32" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1096</v>
       </c>
       <c r="E32" s="22">
+        <f t="shared" si="7"/>
+        <v>7.5616438356164384E-2</v>
+      </c>
+      <c r="F32" s="15">
+        <f t="shared" si="8"/>
+        <v>25281.675616438355</v>
+      </c>
+      <c r="G32" s="29">
+        <v>2</v>
+      </c>
+      <c r="H32" s="25">
+        <f>G32*E32*B32</f>
+        <v>55.351232876712331</v>
+      </c>
+      <c r="I32" s="11">
         <f t="shared" si="5"/>
-        <v>7.5616438356164384E-2</v>
-      </c>
-      <c r="F32" s="15">
-        <f t="shared" si="6"/>
-        <v>25281.675616438355</v>
-      </c>
-      <c r="G32" s="29">
-        <v>2</v>
-      </c>
-      <c r="H32" s="25">
-        <f t="shared" si="7"/>
-        <v>55.351232876712331</v>
-      </c>
-      <c r="I32" s="11">
-        <f t="shared" si="3"/>
         <v>25226.324383561641</v>
       </c>
     </row>
@@ -1563,31 +1564,31 @@
         <v>365</v>
       </c>
       <c r="C33" s="14">
-        <f t="shared" ref="C33:C34" si="8">D32+1-B30</f>
+        <f t="shared" ref="C33:C34" si="9">D32+1-B30</f>
         <v>732</v>
       </c>
       <c r="D33" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1096</v>
       </c>
       <c r="E33" s="22">
+        <f t="shared" si="7"/>
+        <v>7.5616438356164384E-2</v>
+      </c>
+      <c r="F33" s="15">
+        <f t="shared" si="8"/>
+        <v>25226.399999999998</v>
+      </c>
+      <c r="G33" s="29">
+        <v>2</v>
+      </c>
+      <c r="H33" s="25">
+        <f>G33*E33*B33</f>
+        <v>55.2</v>
+      </c>
+      <c r="I33" s="11">
         <f t="shared" si="5"/>
-        <v>7.5616438356164384E-2</v>
-      </c>
-      <c r="F33" s="15">
-        <f t="shared" si="6"/>
-        <v>25226.400000000001</v>
-      </c>
-      <c r="G33" s="29">
-        <v>2</v>
-      </c>
-      <c r="H33" s="25">
-        <f t="shared" si="7"/>
-        <v>55.2</v>
-      </c>
-      <c r="I33" s="11">
-        <f t="shared" si="3"/>
-        <v>25171.200000000001</v>
+        <v>25171.199999999997</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1598,31 +1599,31 @@
         <v>365</v>
       </c>
       <c r="C34" s="14">
+        <f t="shared" si="9"/>
+        <v>732</v>
+      </c>
+      <c r="D34" s="14">
+        <f t="shared" si="6"/>
+        <v>1096</v>
+      </c>
+      <c r="E34" s="22">
+        <f t="shared" si="7"/>
+        <v>7.5616438356164384E-2</v>
+      </c>
+      <c r="F34" s="15">
         <f t="shared" si="8"/>
-        <v>732</v>
-      </c>
-      <c r="D34" s="14">
-        <f t="shared" si="4"/>
-        <v>1096</v>
-      </c>
-      <c r="E34" s="22">
+        <v>25226.399999999998</v>
+      </c>
+      <c r="G34" s="29">
+        <v>2</v>
+      </c>
+      <c r="H34" s="25">
+        <f>G34*E34*B34</f>
+        <v>55.2</v>
+      </c>
+      <c r="I34" s="11">
         <f t="shared" si="5"/>
-        <v>7.5616438356164384E-2</v>
-      </c>
-      <c r="F34" s="15">
-        <f t="shared" si="6"/>
-        <v>25226.400000000001</v>
-      </c>
-      <c r="G34" s="29">
-        <v>2</v>
-      </c>
-      <c r="H34" s="25">
-        <f t="shared" si="7"/>
-        <v>55.2</v>
-      </c>
-      <c r="I34" s="11">
-        <f t="shared" si="3"/>
-        <v>25171.200000000001</v>
+        <v>25171.199999999997</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1644,7 +1645,7 @@
       </c>
       <c r="I35" s="28">
         <f>SUM(I29:I34)</f>
-        <v>120777.52438356163</v>
+        <v>120777.52438356164</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1707,11 +1708,11 @@
         <v>2</v>
       </c>
       <c r="D40" s="22">
-        <f t="shared" ref="D40:D44" si="9">$D$21</f>
+        <f t="shared" ref="D40:D44" si="10">$D$21</f>
         <v>0.64438356164383559</v>
       </c>
       <c r="E40" s="15">
-        <f t="shared" ref="E40:E44" si="10">B40*C40*D40</f>
+        <f t="shared" ref="E40:E44" si="11">B40*C40*D40</f>
         <v>470.4</v>
       </c>
       <c r="F40" s="17"/>
@@ -1729,11 +1730,11 @@
         <v>2</v>
       </c>
       <c r="D41" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E41" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>470.4</v>
       </c>
       <c r="F41" s="17"/>
@@ -1751,11 +1752,11 @@
         <v>2</v>
       </c>
       <c r="D42" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E42" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>471.68876712328768</v>
       </c>
       <c r="F42" s="17"/>
@@ -1773,11 +1774,11 @@
         <v>2</v>
       </c>
       <c r="D43" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E43" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>470.4</v>
       </c>
       <c r="F43" s="17"/>
@@ -1795,11 +1796,11 @@
         <v>2</v>
       </c>
       <c r="D44" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E44" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>470.4</v>
       </c>
       <c r="F44" s="17"/>
@@ -1850,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="B49" s="14">
-        <f>G9</f>
+        <f t="shared" ref="B49:B54" si="12">G9</f>
         <v>0</v>
       </c>
       <c r="C49" s="14">
@@ -1870,18 +1871,18 @@
         <v>2</v>
       </c>
       <c r="B50" s="14">
-        <f>G10</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="C50" s="14">
         <v>1</v>
       </c>
       <c r="D50" s="22">
-        <f t="shared" ref="D50:D54" si="11">$D$21</f>
+        <f t="shared" ref="D50:D54" si="13">$D$21</f>
         <v>0.64438356164383559</v>
       </c>
       <c r="E50" s="15">
-        <f t="shared" ref="E50:E54" si="12">B50*C50*D50</f>
+        <f t="shared" ref="E50:E54" si="14">B50*C50*D50</f>
         <v>0.64438356164383559</v>
       </c>
     </row>
@@ -1890,18 +1891,18 @@
         <v>3</v>
       </c>
       <c r="B51" s="14">
-        <f>G11</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C51" s="14">
         <v>1</v>
       </c>
       <c r="D51" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E51" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.2887671232876712</v>
       </c>
     </row>
@@ -1910,18 +1911,18 @@
         <v>4</v>
       </c>
       <c r="B52" s="14">
-        <f>G12</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C52" s="14">
         <v>1</v>
       </c>
       <c r="D52" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E52" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.2887671232876712</v>
       </c>
     </row>
@@ -1930,18 +1931,18 @@
         <v>5</v>
       </c>
       <c r="B53" s="14">
-        <f>G13</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C53" s="14">
         <v>1</v>
       </c>
       <c r="D53" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E53" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.2887671232876712</v>
       </c>
     </row>
@@ -1950,18 +1951,18 @@
         <v>6</v>
       </c>
       <c r="B54" s="14">
-        <f>G14</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C54" s="14">
         <v>1</v>
       </c>
       <c r="D54" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.64438356164383559</v>
       </c>
       <c r="E54" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.2887671232876712</v>
       </c>
     </row>
@@ -2021,11 +2022,11 @@
         <v>5.4E-6</v>
       </c>
       <c r="C60" s="42">
-        <f t="shared" ref="C60:D60" si="13">C59/10000</f>
+        <f t="shared" ref="C60:D60" si="15">C59/10000</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D60" s="42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.2E-5</v>
       </c>
       <c r="E60" s="16"/>
@@ -2054,11 +2055,11 @@
         <v>4.3000000000000001E-7</v>
       </c>
       <c r="C62" s="42">
-        <f t="shared" ref="C62:D62" si="14">C61/10000</f>
+        <f t="shared" ref="C62:D62" si="16">C61/10000</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="D62" s="42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="E62" s="16"/>
@@ -2102,11 +2103,11 @@
         <v>0</v>
       </c>
       <c r="C65" s="15">
-        <f t="shared" ref="C65:D65" si="15">C64*1000</f>
+        <f t="shared" ref="C65:D65" si="17">C64*1000</f>
         <v>10</v>
       </c>
       <c r="D65" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>24</v>
       </c>
       <c r="E65" s="16"/>
@@ -2412,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="E83" s="45">
-        <f t="shared" ref="E83:E85" si="16">C83*D83</f>
+        <f t="shared" ref="E83:E85" si="18">C83*D83</f>
         <v>0</v>
       </c>
       <c r="F83" s="29">
@@ -2424,11 +2425,11 @@
         <v>24</v>
       </c>
       <c r="H83" s="27">
-        <f t="shared" ref="H83:H85" si="17">F83*G83</f>
+        <f t="shared" ref="H83:H85" si="19">F83*G83</f>
         <v>144</v>
       </c>
       <c r="I83" s="46">
-        <f t="shared" ref="I83:I85" si="18">E83+H83</f>
+        <f t="shared" ref="I83:I85" si="20">E83+H83</f>
         <v>144</v>
       </c>
       <c r="J83" s="35" t="s">
@@ -2447,7 +2448,7 @@
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F84" s="29">
@@ -2462,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J84" s="74" t="s">
@@ -2485,7 +2486,7 @@
         <v>4.3000000000000001E-7</v>
       </c>
       <c r="E85" s="45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.8700000000000002E-6</v>
       </c>
       <c r="F85" s="29">
@@ -2495,11 +2496,11 @@
         <v>0</v>
       </c>
       <c r="H85" s="27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I85" s="45">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.8700000000000002E-6</v>
       </c>
       <c r="J85" s="13"/>
@@ -2797,7 +2798,7 @@
         <v>4.3000000000000001E-7</v>
       </c>
       <c r="E105" s="45">
-        <f t="shared" ref="E105" si="19">C105*D105</f>
+        <f t="shared" ref="E105" si="21">C105*D105</f>
         <v>4.3000000000000001E-7</v>
       </c>
       <c r="F105" s="29">
@@ -2807,11 +2808,11 @@
         <v>0</v>
       </c>
       <c r="H105" s="27">
-        <f t="shared" ref="H105" si="20">F105*G105</f>
+        <f t="shared" ref="H105" si="22">F105*G105</f>
         <v>0</v>
       </c>
       <c r="I105" s="45">
-        <f t="shared" ref="I105" si="21">E105+H105</f>
+        <f t="shared" ref="I105" si="23">E105+H105</f>
         <v>4.3000000000000001E-7</v>
       </c>
     </row>
@@ -4713,8 +4714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C88315-D734-4E4D-AA27-C4BC4AE4260A}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4770,7 +4771,7 @@
       </c>
       <c r="B7" s="5">
         <f>DETAILS!I35</f>
-        <v>120777.52438356163</v>
+        <v>120777.52438356164</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4821,7 +4822,7 @@
       </c>
       <c r="B13" s="7">
         <f>SUM(B3:B12)</f>
-        <v>123797.23355885971</v>
+        <v>123797.23355885972</v>
       </c>
     </row>
   </sheetData>
@@ -4831,6 +4832,58 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F00960A-5938-F34B-8FE2-4DDC40952FE5}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.5" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CA7EBF-B5C5-044E-8E4F-BE20A2072284}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>